<commit_message>
Learnings of 16th Nov
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\100DaysOfCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E3FB91-FAFA-4D06-AE19-A56B75C17992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B403F79E-7165-4481-8946-E449189165DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Multithreading-I yet to finish</t>
+  </si>
+  <si>
+    <t>JSON</t>
   </si>
 </sst>
 </file>
@@ -90,9 +93,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -477,6 +481,34 @@
         <v>8</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>44147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>44148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>44149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>44150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>44151</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>